<commit_message>
started on apical ephys project
</commit_message>
<xml_diff>
--- a/excel/short_tall_apical.xlsx
+++ b/excel/short_tall_apical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar\Documents\Github\analysis_projects\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramr\Documents\Github\analysis_projects\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F245711-5176-4D07-92B1-FB2AB57884E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0DF720-099C-4894-9C17-7E016D89EE06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7C2012AD-026B-49B1-8FAE-912DFF3AF35D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C2012AD-026B-49B1-8FAE-912DFF3AF35D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="35">
   <si>
     <t>Morpho type</t>
   </si>
@@ -73,9 +71,6 @@
   </si>
   <si>
     <t>724539260</t>
-  </si>
-  <si>
-    <t>Tall</t>
   </si>
   <si>
     <t>863404974</t>
@@ -226,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,6 +231,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B07E0AD-B849-4AE6-BE8D-6A685E58F0F0}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="44" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -582,271 +580,265 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="3">
-        <v>969200089</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -854,10 +846,10 @@
         <v>31</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
@@ -865,10 +857,10 @@
         <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -876,30 +868,96 @@
         <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3">
+        <v>969200089</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -914,159 +972,159 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>969200089</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1084,6 +1142,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100337DFFD52317CD448FE74BEAF709F969" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48f5c3690c11efb7595d4b2e6e5b151b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2ab140b7-769f-4ec8-b366-be25b68c27b8" xmlns:ns4="8c40ebc0-3633-427c-8ff8-3ffa936747d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88b539de45d92faf072187374af7f094" ns3:_="" ns4:_="">
     <xsd:import namespace="2ab140b7-769f-4ec8-b366-be25b68c27b8"/>
@@ -1300,12 +1364,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DECF7600-4D0F-4910-82E4-0DECE4F0A8E1}">
   <ds:schemaRefs>
@@ -1315,6 +1373,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F323098-B6D3-4CB2-A250-AFB92F547FFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C47349-BA69-415E-846D-14950C0AA9DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1331,13 +1398,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F323098-B6D3-4CB2-A250-AFB92F547FFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>